<commit_message>
Z3&mysolver result on Arith
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -890,7 +890,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1000,6 +1000,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1445,22 +1448,18 @@
         <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D3" s="3">
-        <v>3.6</v>
-      </c>
-      <c r="E3" s="3">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3">
-        <v>4.4</v>
-      </c>
+        <v>0.6</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="3">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H3" s="8">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="K3" s="28" t="s">
         <v>6</v>
@@ -1493,17 +1492,13 @@
         <v>9</v>
       </c>
       <c r="C4" s="7">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="7">
-        <v>29</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="7">
         <v>49</v>
       </c>
@@ -1543,10 +1538,10 @@
       <c r="E5" s="31"/>
       <c r="F5" s="33"/>
       <c r="G5" s="7">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H5" s="34">
-        <v>9.4</v>
+        <v>10.4</v>
       </c>
       <c r="K5" s="29"/>
       <c r="L5" s="31" t="s">
@@ -1569,12 +1564,10 @@
         <v>11</v>
       </c>
       <c r="C6" s="6">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D6" s="6"/>
-      <c r="E6" s="6">
-        <v>61</v>
-      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6">
         <v>0</v>
@@ -1605,22 +1598,18 @@
         <v>7</v>
       </c>
       <c r="C7" s="3">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3">
-        <v>8.6</v>
-      </c>
-      <c r="E7" s="3">
-        <v>3</v>
-      </c>
-      <c r="F7" s="35" t="s">
-        <v>8</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="35"/>
       <c r="G7" s="3">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H7" s="8">
-        <v>8.54</v>
+        <v>3.5</v>
       </c>
       <c r="K7" s="28" t="s">
         <v>12</v>
@@ -1658,14 +1647,10 @@
       <c r="D8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="7">
-        <v>26</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="7">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>8</v>
@@ -1703,9 +1688,11 @@
       <c r="E9" s="31"/>
       <c r="F9" s="33"/>
       <c r="G9" s="7">
-        <v>0</v>
-      </c>
-      <c r="H9" s="36"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="36">
+        <v>53.8</v>
+      </c>
       <c r="K9" s="29"/>
       <c r="L9" s="31" t="s">
         <v>10</v>
@@ -1727,15 +1714,13 @@
         <v>11</v>
       </c>
       <c r="C10" s="6">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="6">
-        <v>71</v>
-      </c>
+      <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H10" s="9"/>
       <c r="K10" s="32"/>
@@ -1763,24 +1748,20 @@
         <v>7</v>
       </c>
       <c r="C11" s="3">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D11" s="3">
-        <v>3.6</v>
-      </c>
-      <c r="E11" s="3">
-        <v>5</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.2</v>
-      </c>
+        <v>1.8</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="3">
-        <v>18</v>
-      </c>
-      <c r="H11" s="8">
-        <v>17.5</v>
-      </c>
-      <c r="K11" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="37">
+        <v>20</v>
+      </c>
+      <c r="K11" s="38" t="s">
         <v>14</v>
       </c>
       <c r="L11" s="3" t="s">
@@ -1811,24 +1792,20 @@
         <v>9</v>
       </c>
       <c r="C12" s="7">
-        <v>16</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="7">
-        <v>16</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>8</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="7">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H12" s="11">
         <v>0.1</v>
       </c>
-      <c r="K12" s="38"/>
+      <c r="K12" s="39"/>
       <c r="L12" s="7" t="s">
         <v>9</v>
       </c>
@@ -1864,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="36"/>
-      <c r="K13" s="38"/>
+      <c r="K13" s="39"/>
       <c r="L13" s="31" t="s">
         <v>10</v>
       </c>
@@ -1885,18 +1862,16 @@
         <v>11</v>
       </c>
       <c r="C14" s="6">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="6">
-        <v>79</v>
-      </c>
+      <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="H14" s="9"/>
-      <c r="K14" s="39"/>
+      <c r="K14" s="40"/>
       <c r="L14" s="6" t="s">
         <v>11</v>
       </c>
@@ -1997,7 +1972,12 @@
       </c>
       <c r="R18" s="9"/>
     </row>
-    <row r="21" spans="13:19">
+    <row r="20" spans="7:7">
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="7:19">
+      <c r="G21"/>
+      <c r="H21"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1" t="s">
         <v>0</v>
@@ -2012,7 +1992,9 @@
       </c>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="13:19">
+    <row r="22" spans="7:19">
+      <c r="G22"/>
+      <c r="H22"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1" t="s">
         <v>4</v>
@@ -2033,7 +2015,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="11:19">
+    <row r="23" spans="7:19">
+      <c r="G23"/>
+      <c r="H23"/>
       <c r="K23" s="2" t="s">
         <v>15</v>
       </c>
@@ -2211,7 +2195,7 @@
     </row>
     <row r="31" spans="11:19">
       <c r="K31" s="4"/>
-      <c r="L31" s="37" t="s">
+      <c r="L31" s="38" t="s">
         <v>14</v>
       </c>
       <c r="M31" s="3" t="s">
@@ -2232,7 +2216,7 @@
     </row>
     <row r="32" spans="11:19">
       <c r="K32" s="4"/>
-      <c r="L32" s="38"/>
+      <c r="L32" s="39"/>
       <c r="M32" s="7" t="s">
         <v>9</v>
       </c>
@@ -2257,7 +2241,7 @@
     </row>
     <row r="33" spans="11:19">
       <c r="K33" s="4"/>
-      <c r="L33" s="38"/>
+      <c r="L33" s="39"/>
       <c r="M33" s="31" t="s">
         <v>10</v>
       </c>
@@ -2274,7 +2258,7 @@
     </row>
     <row r="34" spans="11:19">
       <c r="K34" s="4"/>
-      <c r="L34" s="39"/>
+      <c r="L34" s="40"/>
       <c r="M34" s="6" t="s">
         <v>11</v>
       </c>
@@ -2387,7 +2371,7 @@
       <c r="K39" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="L39" s="40" t="s">
+      <c r="L39" s="41" t="s">
         <v>6</v>
       </c>
       <c r="M39" s="5" t="s">
@@ -2396,7 +2380,7 @@
       <c r="N39" s="2">
         <v>31</v>
       </c>
-      <c r="O39" s="42" t="s">
+      <c r="O39" s="43" t="s">
         <v>8</v>
       </c>
       <c r="P39" s="3">
@@ -2405,7 +2389,7 @@
       <c r="Q39" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R39" s="42">
+      <c r="R39" s="43">
         <v>37</v>
       </c>
       <c r="S39" s="8" t="s">
@@ -2414,8 +2398,8 @@
     </row>
     <row r="40" spans="11:19">
       <c r="K40" s="29"/>
-      <c r="L40" s="40"/>
-      <c r="M40" s="43" t="s">
+      <c r="L40" s="41"/>
+      <c r="M40" s="44" t="s">
         <v>9</v>
       </c>
       <c r="N40" s="4">
@@ -2430,17 +2414,17 @@
       <c r="Q40" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="R40" s="44">
+      <c r="R40" s="45">
         <v>46</v>
       </c>
-      <c r="S40" s="45" t="s">
+      <c r="S40" s="46" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="11:19">
       <c r="K41" s="29"/>
-      <c r="L41" s="40"/>
-      <c r="M41" s="43" t="s">
+      <c r="L41" s="41"/>
+      <c r="M41" s="44" t="s">
         <v>10</v>
       </c>
       <c r="N41" s="4"/>
@@ -2456,8 +2440,8 @@
     </row>
     <row r="42" spans="11:19">
       <c r="K42" s="29"/>
-      <c r="L42" s="40"/>
-      <c r="M42" s="43" t="s">
+      <c r="L42" s="41"/>
+      <c r="M42" s="44" t="s">
         <v>11</v>
       </c>
       <c r="N42" s="5">
@@ -2468,17 +2452,17 @@
         <v>56</v>
       </c>
       <c r="Q42" s="6"/>
-      <c r="R42" s="46">
+      <c r="R42" s="47">
         <v>0</v>
       </c>
       <c r="S42" s="9"/>
     </row>
     <row r="43" spans="11:19">
       <c r="K43" s="29"/>
-      <c r="L43" s="40" t="s">
+      <c r="L43" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="M43" s="43" t="s">
+      <c r="M43" s="44" t="s">
         <v>7</v>
       </c>
       <c r="N43" s="2">
@@ -2490,10 +2474,10 @@
       <c r="P43" s="3">
         <v>13</v>
       </c>
-      <c r="Q43" s="42" t="s">
+      <c r="Q43" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="R43" s="42">
+      <c r="R43" s="43">
         <v>36</v>
       </c>
       <c r="S43" s="8">
@@ -2502,8 +2486,8 @@
     </row>
     <row r="44" spans="11:19">
       <c r="K44" s="29"/>
-      <c r="L44" s="40"/>
-      <c r="M44" s="43" t="s">
+      <c r="L44" s="41"/>
+      <c r="M44" s="44" t="s">
         <v>9</v>
       </c>
       <c r="N44" s="4">
@@ -2518,17 +2502,17 @@
       <c r="Q44" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="R44" s="44">
+      <c r="R44" s="45">
         <v>42</v>
       </c>
-      <c r="S44" s="45" t="s">
+      <c r="S44" s="46" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="45" spans="11:19">
       <c r="K45" s="29"/>
-      <c r="L45" s="40"/>
-      <c r="M45" s="43" t="s">
+      <c r="L45" s="41"/>
+      <c r="M45" s="44" t="s">
         <v>10</v>
       </c>
       <c r="N45" s="4"/>
@@ -2544,8 +2528,8 @@
     </row>
     <row r="46" spans="11:19">
       <c r="K46" s="29"/>
-      <c r="L46" s="40"/>
-      <c r="M46" s="43" t="s">
+      <c r="L46" s="41"/>
+      <c r="M46" s="44" t="s">
         <v>11</v>
       </c>
       <c r="N46" s="5">
@@ -2556,23 +2540,23 @@
         <v>67</v>
       </c>
       <c r="Q46" s="6"/>
-      <c r="R46" s="46">
+      <c r="R46" s="47">
         <v>19</v>
       </c>
       <c r="S46" s="9"/>
     </row>
     <row r="47" spans="11:19">
       <c r="K47" s="29"/>
-      <c r="L47" s="41" t="s">
+      <c r="L47" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="M47" s="40" t="s">
+      <c r="M47" s="41" t="s">
         <v>7</v>
       </c>
       <c r="N47" s="7">
         <v>3</v>
       </c>
-      <c r="O47" s="44">
+      <c r="O47" s="45">
         <v>23</v>
       </c>
       <c r="P47" s="7">
@@ -2581,7 +2565,7 @@
       <c r="Q47" s="7">
         <v>39</v>
       </c>
-      <c r="R47" s="44">
+      <c r="R47" s="45">
         <v>14</v>
       </c>
       <c r="S47" s="11">
@@ -2590,8 +2574,8 @@
     </row>
     <row r="48" spans="11:19">
       <c r="K48" s="29"/>
-      <c r="L48" s="40"/>
-      <c r="M48" s="40" t="s">
+      <c r="L48" s="41"/>
+      <c r="M48" s="41" t="s">
         <v>9</v>
       </c>
       <c r="N48" s="1">
@@ -2609,14 +2593,14 @@
       <c r="R48" s="10">
         <v>47</v>
       </c>
-      <c r="S48" s="45" t="s">
+      <c r="S48" s="46" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="49" spans="11:19">
       <c r="K49" s="29"/>
-      <c r="L49" s="40"/>
-      <c r="M49" s="40" t="s">
+      <c r="L49" s="41"/>
+      <c r="M49" s="41" t="s">
         <v>10</v>
       </c>
       <c r="N49" s="1"/>
@@ -2632,8 +2616,8 @@
     </row>
     <row r="50" spans="11:19">
       <c r="K50" s="29"/>
-      <c r="L50" s="40"/>
-      <c r="M50" s="40" t="s">
+      <c r="L50" s="41"/>
+      <c r="M50" s="41" t="s">
         <v>11</v>
       </c>
       <c r="N50" s="6">
@@ -2644,20 +2628,20 @@
         <v>74</v>
       </c>
       <c r="Q50" s="6"/>
-      <c r="R50" s="46">
+      <c r="R50" s="47">
         <v>37</v>
       </c>
       <c r="S50" s="9"/>
     </row>
     <row r="51" spans="11:19">
       <c r="K51" s="29"/>
-      <c r="L51" s="40" t="s">
+      <c r="L51" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="M51" s="40" t="s">
+      <c r="M51" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="N51" s="42">
+      <c r="N51" s="43">
         <v>29</v>
       </c>
       <c r="O51" s="3">
@@ -2666,7 +2650,7 @@
       <c r="P51" s="3">
         <v>11</v>
       </c>
-      <c r="Q51" s="42" t="s">
+      <c r="Q51" s="43" t="s">
         <v>8</v>
       </c>
       <c r="R51" s="3">
@@ -2678,8 +2662,8 @@
     </row>
     <row r="52" spans="11:19">
       <c r="K52" s="29"/>
-      <c r="L52" s="40"/>
-      <c r="M52" s="40" t="s">
+      <c r="L52" s="41"/>
+      <c r="M52" s="41" t="s">
         <v>9</v>
       </c>
       <c r="N52" s="7">
@@ -2694,17 +2678,17 @@
       <c r="Q52" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="R52" s="44">
+      <c r="R52" s="45">
         <v>38</v>
       </c>
-      <c r="S52" s="45" t="s">
+      <c r="S52" s="46" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="53" spans="11:19">
       <c r="K53" s="29"/>
-      <c r="L53" s="40"/>
-      <c r="M53" s="40" t="s">
+      <c r="L53" s="41"/>
+      <c r="M53" s="41" t="s">
         <v>10</v>
       </c>
       <c r="N53" s="7"/>
@@ -2716,8 +2700,8 @@
     </row>
     <row r="54" spans="11:19">
       <c r="K54" s="32"/>
-      <c r="L54" s="40"/>
-      <c r="M54" s="40" t="s">
+      <c r="L54" s="41"/>
+      <c r="M54" s="41" t="s">
         <v>11</v>
       </c>
       <c r="N54" s="6">
@@ -2728,7 +2712,7 @@
         <v>69</v>
       </c>
       <c r="Q54" s="6"/>
-      <c r="R54" s="46">
+      <c r="R54" s="47">
         <v>34</v>
       </c>
       <c r="S54" s="9"/>

</xml_diff>